<commit_message>
feat: add additional-configuration to excelSync
</commit_message>
<xml_diff>
--- a/Connectors-Template.xlsx
+++ b/Connectors-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tnotheis\src\enmeshed\connector-manager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkoenig/git/nmshd/connector-manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51059A9-F14F-4DDD-94CF-A4DE1D7EB393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07098E3D-EE3C-BE47-B215-0178867344B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="520" windowWidth="51220" windowHeight="26920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>backbone-base-url</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>connector-version</t>
+  </si>
+  <si>
+    <t>additional-configuration</t>
   </si>
 </sst>
 </file>
@@ -115,8 +118,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -132,12 +135,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0">
-  <autoFilter ref="A1:H2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:I2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:I2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H2">
     <sortCondition descending="1" ref="B1:B2"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{33890D53-6763-4B54-8B8D-BCAC9A2EF139}" name="connector-id"/>
     <tableColumn id="2" xr3:uid="{272DDE2C-8254-4855-B433-2FFA394DB9A4}" name="connector-port"/>
     <tableColumn id="3" xr3:uid="{AC9F5FBE-4F34-404D-95B3-82665C59D054}" name="connector-version"/>
@@ -146,6 +149,7 @@
     <tableColumn id="6" xr3:uid="{5ECBF7AF-F3AC-4261-90A2-0ED6E97AF822}" name="backbone-base-url"/>
     <tableColumn id="7" xr3:uid="{425BDFAA-D4D8-4118-8C96-99FBDA1C3AF9}" name="backbone-client-id"/>
     <tableColumn id="8" xr3:uid="{6733AEFD-8C51-4384-98A4-D63990EC25F4}" name="backbone-client-secret"/>
+    <tableColumn id="9" xr3:uid="{8A869A99-489E-5348-AA80-47E74F0F8912}" name="additional-configuration"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -414,25 +418,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -457,13 +462,17 @@
       <c r="H1" t="s">
         <v>2</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -472,22 +481,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A291A44-47E4-425E-963E-799631E19E58}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -503,8 +514,11 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove DisplayName attribute setting (#5)
* feat: add description

* feat: add description

* refactor: use description instead of displayName
</commit_message>
<xml_diff>
--- a/Connectors-Template.xlsx
+++ b/Connectors-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tnotheis\src\enmeshed\connector-manager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkoenig/git/nmshd/connector-manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51059A9-F14F-4DDD-94CF-A4DE1D7EB393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E744D0FB-D707-E245-9F60-20E0BCEBC075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50660" yWindow="500" windowWidth="51740" windowHeight="26920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -46,10 +46,10 @@
     <t>connector-id</t>
   </si>
   <si>
-    <t>organization-display-name</t>
-  </si>
-  <si>
     <t>connector-version</t>
+  </si>
+  <si>
+    <t>connector-description</t>
   </si>
 </sst>
 </file>
@@ -115,8 +115,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -135,14 +135,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0">
   <autoFilter ref="A1:H2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H2">
-    <sortCondition descending="1" ref="B1:B2"/>
+    <sortCondition descending="1" ref="C1:C2"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{33890D53-6763-4B54-8B8D-BCAC9A2EF139}" name="connector-id"/>
+    <tableColumn id="9" xr3:uid="{647EB3D6-D324-1D48-9F94-8ABCC19E5887}" name="connector-description"/>
     <tableColumn id="2" xr3:uid="{272DDE2C-8254-4855-B433-2FFA394DB9A4}" name="connector-port"/>
     <tableColumn id="3" xr3:uid="{AC9F5FBE-4F34-404D-95B3-82665C59D054}" name="connector-version"/>
     <tableColumn id="4" xr3:uid="{2A3E0870-F1A2-4ED3-93F5-970AB21EA06D}" name="connector-db-connection-string"/>
-    <tableColumn id="5" xr3:uid="{15AB552C-92FD-418C-9F0A-DF7C51E90D08}" name="organization-display-name"/>
     <tableColumn id="6" xr3:uid="{5ECBF7AF-F3AC-4261-90A2-0ED6E97AF822}" name="backbone-base-url"/>
     <tableColumn id="7" xr3:uid="{425BDFAA-D4D8-4118-8C96-99FBDA1C3AF9}" name="backbone-client-id"/>
     <tableColumn id="8" xr3:uid="{6733AEFD-8C51-4384-98A4-D63990EC25F4}" name="backbone-client-secret"/>
@@ -417,36 +417,36 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -458,12 +458,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="3"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -478,21 +479,21 @@
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -504,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
     </row>
   </sheetData>

</xml_diff>